<commit_message>
cap nhat import xe, giao vien
</commit_message>
<xml_diff>
--- a/web/xe.xlsx
+++ b/web/xe.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CV\2024\TruongLai\pmDaoTao\quanlydaotao\web\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2865A843-BFD8-447F-B663-82D8AD7109D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2157519-25B4-4349-9163-D97FC9176E12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4F3FFC8B-0BD8-4B19-948E-9890A9638651}"/>
   </bookViews>
@@ -1321,8 +1321,8 @@
   </sheetPr>
   <dimension ref="A1:O92"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F74" sqref="F74"/>
+    <sheetView tabSelected="1" topLeftCell="A77" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="E97" sqref="E97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
cap nhat hoa don
</commit_message>
<xml_diff>
--- a/web/xe.xlsx
+++ b/web/xe.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CV\2024\TruongLai\pmDaoTao\quanlydaotao\web\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D2C5F51-6778-4ECD-9835-362805952E6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F8D2CB7-B8AB-42EC-BF8E-7C75E799C986}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4F3FFC8B-0BD8-4B19-948E-9890A9638651}"/>
   </bookViews>
@@ -16,14 +16,14 @@
     <sheet name="TÀI SẢN XE" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'TÀI SẢN XE'!$A$1:$N$11</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'TÀI SẢN XE'!$A$1:$N$1</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="76">
   <si>
     <t>STT</t>
   </si>
@@ -170,6 +170,87 @@
   </si>
   <si>
     <t>84A-201.44</t>
+  </si>
+  <si>
+    <t>Ô-TÔ CON VIOS 1.5E CVT</t>
+  </si>
+  <si>
+    <t>RL4B28F38S5350910</t>
+  </si>
+  <si>
+    <t>2NRY455288</t>
+  </si>
+  <si>
+    <t>84A-243.37</t>
+  </si>
+  <si>
+    <t>CÔNG TY TNHH TOYOTA THẬP NHẤT PHONG VĨNH LONG</t>
+  </si>
+  <si>
+    <t>15A-05/HĐMB-TVL/25</t>
+  </si>
+  <si>
+    <t>RL4B28F30S5350514</t>
+  </si>
+  <si>
+    <t>2NRY443395</t>
+  </si>
+  <si>
+    <t>84A-243.48</t>
+  </si>
+  <si>
+    <t>Ô-TÔ TẢI FUSO</t>
+  </si>
+  <si>
+    <t>RNHA13SSBLC016958</t>
+  </si>
+  <si>
+    <t>400924D0026768</t>
+  </si>
+  <si>
+    <t>84A-244.57</t>
+  </si>
+  <si>
+    <t>RNHA13SSBLC016961</t>
+  </si>
+  <si>
+    <t>400924D0026744</t>
+  </si>
+  <si>
+    <t>84A-245.12</t>
+  </si>
+  <si>
+    <t>Ô-TÔ HUYNDAI</t>
+  </si>
+  <si>
+    <t>RPPHG17PPED000319</t>
+  </si>
+  <si>
+    <t>D4DDE562379</t>
+  </si>
+  <si>
+    <t>84A-245.20</t>
+  </si>
+  <si>
+    <t>RRFHDI7PPFT003695</t>
+  </si>
+  <si>
+    <t>D4DDEJ585731</t>
+  </si>
+  <si>
+    <t>84A-244.74</t>
+  </si>
+  <si>
+    <t>CNHTC (Bồn bê tông)</t>
+  </si>
+  <si>
+    <t>LZZ5CCMC1FN074736</t>
+  </si>
+  <si>
+    <t>WD61562150417 004407</t>
+  </si>
+  <si>
+    <t>84A-243.75</t>
   </si>
 </sst>
 </file>
@@ -177,8 +258,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="168" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -215,7 +296,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -225,6 +306,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -255,20 +348,32 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Comma 2" xfId="1" xr:uid="{50005E9D-67E4-45AF-B1DF-39D7E3C2EFC8}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -550,10 +655,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:O11"/>
+  <dimension ref="A1:O18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -620,408 +725,658 @@
       </c>
       <c r="O1" s="2"/>
     </row>
-    <row r="2" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
         <v>1</v>
       </c>
       <c r="B2" s="4">
-        <v>4</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H2" s="5"/>
-      <c r="I2" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="J2" s="4">
+        <v>3</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="G2" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="8"/>
+      <c r="I2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="J2" s="5">
         <v>0</v>
       </c>
       <c r="K2" s="6">
-        <v>425000000</v>
+        <v>468000000</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="M2" s="5"/>
+        <v>53</v>
+      </c>
+      <c r="M2" s="3"/>
       <c r="N2" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
-        <v>1</v>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="18">
+        <v>2</v>
       </c>
       <c r="B3" s="4">
-        <v>4</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H3" s="5"/>
-      <c r="I3" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="J3" s="4">
+        <v>3</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="G3" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="8"/>
+      <c r="I3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="J3" s="18">
         <v>0</v>
       </c>
       <c r="K3" s="6">
-        <v>425000000</v>
+        <v>468000000</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="M3" s="5"/>
+        <v>53</v>
+      </c>
+      <c r="M3" s="3"/>
       <c r="N3" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
-        <v>1</v>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="18">
+        <v>3</v>
       </c>
       <c r="B4" s="4">
         <v>4</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H4" s="5"/>
-      <c r="I4" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="J4" s="4">
+      <c r="D4" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" s="7"/>
+      <c r="I4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="J4" s="18">
         <v>0</v>
       </c>
       <c r="K4" s="6">
         <v>425000000</v>
       </c>
-      <c r="L4" s="4" t="s">
+      <c r="L4" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="M4" s="5"/>
-      <c r="N4" s="4" t="s">
+      <c r="M4" s="3"/>
+      <c r="N4" s="5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
-        <v>1</v>
-      </c>
-      <c r="B5" s="4">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="18">
         <v>4</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="B5" s="17">
+        <v>4</v>
+      </c>
+      <c r="C5" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H5" s="5"/>
-      <c r="I5" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="J5" s="4">
+      <c r="D5" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" s="7"/>
+      <c r="I5" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="J5" s="18">
         <v>0</v>
       </c>
       <c r="K5" s="6">
         <v>425000000</v>
       </c>
-      <c r="L5" s="4" t="s">
+      <c r="L5" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="M5" s="5"/>
-      <c r="N5" s="4" t="s">
+      <c r="M5" s="3"/>
+      <c r="N5" s="5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
-        <v>1</v>
-      </c>
-      <c r="B6" s="4">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="18">
+        <v>5</v>
+      </c>
+      <c r="B6" s="17">
         <v>4</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H6" s="5"/>
-      <c r="I6" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="J6" s="4">
+      <c r="D6" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G6" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" s="7"/>
+      <c r="I6" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="J6" s="18">
         <v>0</v>
       </c>
       <c r="K6" s="6">
         <v>425000000</v>
       </c>
-      <c r="L6" s="4" t="s">
+      <c r="L6" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="M6" s="5"/>
-      <c r="N6" s="4" t="s">
+      <c r="M6" s="3"/>
+      <c r="N6" s="5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="4">
-        <v>1</v>
-      </c>
-      <c r="B7" s="4">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="18">
+        <v>6</v>
+      </c>
+      <c r="B7" s="17">
         <v>4</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H7" s="5"/>
-      <c r="I7" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="J7" s="4">
+      <c r="D7" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="G7" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7" s="7"/>
+      <c r="I7" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="J7" s="18">
         <v>0</v>
       </c>
       <c r="K7" s="6">
         <v>425000000</v>
       </c>
-      <c r="L7" s="4" t="s">
+      <c r="L7" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="M7" s="5"/>
-      <c r="N7" s="4" t="s">
+      <c r="M7" s="3"/>
+      <c r="N7" s="5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="4">
-        <v>1</v>
-      </c>
-      <c r="B8" s="4">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="18">
+        <v>7</v>
+      </c>
+      <c r="B8" s="17">
         <v>4</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H8" s="5"/>
-      <c r="I8" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="J8" s="4">
+      <c r="D8" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="G8" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="H8" s="7"/>
+      <c r="I8" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="J8" s="18">
         <v>0</v>
       </c>
       <c r="K8" s="6">
         <v>425000000</v>
       </c>
-      <c r="L8" s="4" t="s">
+      <c r="L8" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="M8" s="5"/>
-      <c r="N8" s="4" t="s">
+      <c r="M8" s="3"/>
+      <c r="N8" s="5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="4">
-        <v>1</v>
-      </c>
-      <c r="B9" s="4">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="18">
+        <v>8</v>
+      </c>
+      <c r="B9" s="17">
         <v>4</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H9" s="5"/>
-      <c r="I9" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="J9" s="4">
+      <c r="D9" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="G9" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="H9" s="7"/>
+      <c r="I9" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="J9" s="18">
         <v>0</v>
       </c>
       <c r="K9" s="6">
         <v>425000000</v>
       </c>
-      <c r="L9" s="4" t="s">
+      <c r="L9" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="M9" s="5"/>
-      <c r="N9" s="4" t="s">
+      <c r="M9" s="3"/>
+      <c r="N9" s="5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="4">
-        <v>1</v>
-      </c>
-      <c r="B10" s="4">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="18">
+        <v>9</v>
+      </c>
+      <c r="B10" s="17">
         <v>4</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H10" s="5"/>
-      <c r="I10" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="J10" s="4">
+      <c r="D10" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="G10" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="H10" s="7"/>
+      <c r="I10" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="J10" s="18">
         <v>0</v>
       </c>
       <c r="K10" s="6">
         <v>425000000</v>
       </c>
-      <c r="L10" s="4" t="s">
+      <c r="L10" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="M10" s="5"/>
-      <c r="N10" s="4" t="s">
+      <c r="M10" s="3"/>
+      <c r="N10" s="5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="4">
-        <v>1</v>
-      </c>
-      <c r="B11" s="4">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="18">
+        <v>10</v>
+      </c>
+      <c r="B11" s="17">
         <v>4</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H11" s="5"/>
-      <c r="I11" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="J11" s="4">
+      <c r="D11" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="G11" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="H11" s="7"/>
+      <c r="I11" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="J11" s="18">
         <v>0</v>
       </c>
       <c r="K11" s="6">
         <v>425000000</v>
       </c>
-      <c r="L11" s="4" t="s">
+      <c r="L11" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="M11" s="5"/>
-      <c r="N11" s="4" t="s">
+      <c r="M11" s="3"/>
+      <c r="N11" s="5" t="s">
         <v>21</v>
       </c>
     </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="18">
+        <v>11</v>
+      </c>
+      <c r="B12" s="17">
+        <v>4</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="G12" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="H12" s="7"/>
+      <c r="I12" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="J12" s="18">
+        <v>0</v>
+      </c>
+      <c r="K12" s="6">
+        <v>425000000</v>
+      </c>
+      <c r="L12" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="M12" s="3"/>
+      <c r="N12" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" s="18">
+        <v>12</v>
+      </c>
+      <c r="B13" s="17">
+        <v>4</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="G13" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="H13" s="7"/>
+      <c r="I13" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="J13" s="18">
+        <v>0</v>
+      </c>
+      <c r="K13" s="6">
+        <v>425000000</v>
+      </c>
+      <c r="L13" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="M13" s="3"/>
+      <c r="N13" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" s="18">
+        <v>13</v>
+      </c>
+      <c r="B14" s="17">
+        <v>4</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="F14" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="G14" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="H14" s="11"/>
+      <c r="I14" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="J14" s="18">
+        <v>0</v>
+      </c>
+      <c r="K14" s="13">
+        <v>765000000</v>
+      </c>
+      <c r="L14" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="M14" s="11">
+        <v>2675</v>
+      </c>
+      <c r="N14" s="11"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" s="18">
+        <v>14</v>
+      </c>
+      <c r="B15" s="17">
+        <v>4</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="E15" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="F15" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="G15" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="H15" s="11"/>
+      <c r="I15" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="J15" s="18">
+        <v>0</v>
+      </c>
+      <c r="K15" s="13">
+        <v>765000001</v>
+      </c>
+      <c r="L15" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="M15" s="11">
+        <v>2676</v>
+      </c>
+      <c r="N15" s="11"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" s="18">
+        <v>15</v>
+      </c>
+      <c r="B16" s="16">
+        <v>1</v>
+      </c>
+      <c r="C16" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="D16" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="E16" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="F16" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="G16" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="H16" s="16"/>
+      <c r="I16" s="16"/>
+      <c r="J16" s="18"/>
+      <c r="K16" s="16"/>
+      <c r="L16" s="16"/>
+      <c r="M16" s="16"/>
+      <c r="N16" s="16"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A17" s="18">
+        <v>16</v>
+      </c>
+      <c r="B17" s="16">
+        <v>1</v>
+      </c>
+      <c r="C17" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="D17" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="E17" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="F17" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="G17" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="H17" s="16"/>
+      <c r="I17" s="16"/>
+      <c r="J17" s="18"/>
+      <c r="K17" s="16"/>
+      <c r="L17" s="16"/>
+      <c r="M17" s="16"/>
+      <c r="N17" s="16"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A18" s="18">
+        <v>17</v>
+      </c>
+      <c r="B18" s="16">
+        <v>1</v>
+      </c>
+      <c r="C18" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="D18" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="E18" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="F18" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="G18" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="H18" s="16"/>
+      <c r="I18" s="16"/>
+      <c r="J18" s="18"/>
+      <c r="K18" s="16"/>
+      <c r="L18" s="16"/>
+      <c r="M18" s="16"/>
+      <c r="N18" s="16"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:N11" xr:uid="{BC0830FC-077D-4FB9-ACA1-1741738619A0}"/>
+  <autoFilter ref="A1:N1" xr:uid="{BC0830FC-077D-4FB9-ACA1-1741738619A0}"/>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup scale="97" fitToHeight="0" orientation="landscape" r:id="rId1"/>
 </worksheet>

</xml_diff>